<commit_message>
update code whcih can automatically extract data from website
</commit_message>
<xml_diff>
--- a/data/NBA-Play-by-Play Data_Sample/(2016-06-10)-0041500404-GSW@CLE.xlsx
+++ b/data/NBA-Play-by-Play Data_Sample/(2016-06-10)-0041500404-GSW@CLE.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17830"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11013"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\downloads\sample-pbp-log\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaelyang/Dropbox/Lab/sport/data/NBA-Play-by-Play Data_Sample/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DC5BA42-6638-5E48-B447-72F1BCCEB586}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7935"/>
+    <workbookView xWindow="8980" yWindow="3020" windowWidth="33480" windowHeight="17880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="(2016-06-10)-0041500404-GSW@CLE" sheetId="1" r:id="rId1"/>
@@ -18,7 +19,15 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'(2016-06-10)-0041500404-GSW@CLE'!$A$2:$AR$469</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -1775,7 +1784,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2661,51 +2670,51 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AR469"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="F1" sqref="F1"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="AD445" sqref="AD445"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="10.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="8.1328125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="9.1328125" style="1"/>
-    <col min="3" max="3" width="8.73046875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.59765625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.3984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.73046875" style="1" customWidth="1"/>
-    <col min="7" max="8" width="16.86328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.59765625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.1328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.1640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.1640625" style="1"/>
+    <col min="3" max="3" width="8.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.6640625" style="1" customWidth="1"/>
+    <col min="7" max="8" width="16.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="13" width="16" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.73046875" style="1" customWidth="1"/>
-    <col min="15" max="16" width="13.59765625" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="14.59765625" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.1328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.6640625" style="1" customWidth="1"/>
+    <col min="15" max="16" width="13.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="7.9296875" style="1" customWidth="1"/>
-    <col min="21" max="21" width="7.265625" style="1" customWidth="1"/>
+    <col min="20" max="20" width="8" style="1" customWidth="1"/>
+    <col min="21" max="21" width="7.33203125" style="1" customWidth="1"/>
     <col min="22" max="22" width="11" style="1" customWidth="1"/>
-    <col min="23" max="24" width="9.1328125" style="1"/>
-    <col min="25" max="25" width="10.46484375" style="1" customWidth="1"/>
-    <col min="26" max="31" width="9.1328125" style="1"/>
-    <col min="32" max="32" width="11.06640625" style="1" customWidth="1"/>
-    <col min="33" max="37" width="9.1328125" style="1"/>
-    <col min="38" max="38" width="8.46484375" style="1" customWidth="1"/>
-    <col min="39" max="39" width="13.265625" style="1" customWidth="1"/>
-    <col min="40" max="40" width="13.265625" style="3" customWidth="1"/>
-    <col min="41" max="41" width="13.265625" style="1" customWidth="1"/>
-    <col min="42" max="42" width="22.73046875" style="1" customWidth="1"/>
-    <col min="43" max="43" width="22.796875" style="1" customWidth="1"/>
-    <col min="44" max="44" width="42.73046875" style="1" bestFit="1" customWidth="1"/>
-    <col min="45" max="16384" width="9.1328125" style="1"/>
+    <col min="23" max="24" width="9.1640625" style="1"/>
+    <col min="25" max="25" width="10.5" style="1" customWidth="1"/>
+    <col min="26" max="31" width="9.1640625" style="1"/>
+    <col min="32" max="32" width="11" style="1" customWidth="1"/>
+    <col min="33" max="37" width="9.1640625" style="1"/>
+    <col min="38" max="38" width="8.5" style="1" customWidth="1"/>
+    <col min="39" max="39" width="13.33203125" style="1" customWidth="1"/>
+    <col min="40" max="40" width="13.33203125" style="3" customWidth="1"/>
+    <col min="41" max="41" width="13.33203125" style="1" customWidth="1"/>
+    <col min="42" max="42" width="22.6640625" style="1" customWidth="1"/>
+    <col min="43" max="43" width="22.83203125" style="1" customWidth="1"/>
+    <col min="44" max="44" width="42.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="45" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:44" ht="15.75" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:44" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -2839,7 +2848,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="2" spans="1:44" s="2" customFormat="1" ht="84" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:44" s="2" customFormat="1" ht="96" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>578</v>
       </c>
@@ -2973,7 +2982,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="3" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A3" s="4" t="str">
         <f t="shared" ref="A3:A66" si="0">"0041500404"</f>
         <v>0041500404</v>
@@ -3063,7 +3072,7 @@
       <c r="AQ3" s="4"/>
       <c r="AR3" s="4"/>
     </row>
-    <row r="4" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A4" s="4" t="str">
         <f t="shared" si="0"/>
         <v>0041500404</v>
@@ -3165,7 +3174,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="5" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A5" s="4" t="str">
         <f t="shared" si="0"/>
         <v>0041500404</v>
@@ -3276,7 +3285,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="6" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A6" s="4" t="str">
         <f t="shared" si="0"/>
         <v>0041500404</v>
@@ -3372,7 +3381,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="7" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A7" s="4" t="str">
         <f t="shared" si="0"/>
         <v>0041500404</v>
@@ -3485,7 +3494,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="8" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A8" s="4" t="str">
         <f t="shared" si="0"/>
         <v>0041500404</v>
@@ -3598,7 +3607,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="9" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A9" s="4" t="str">
         <f t="shared" si="0"/>
         <v>0041500404</v>
@@ -3698,7 +3707,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="10" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A10" s="4" t="str">
         <f t="shared" si="0"/>
         <v>0041500404</v>
@@ -3802,7 +3811,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="11" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A11" s="4" t="str">
         <f t="shared" si="0"/>
         <v>0041500404</v>
@@ -3906,7 +3915,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="12" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A12" s="4" t="str">
         <f t="shared" si="0"/>
         <v>0041500404</v>
@@ -4019,7 +4028,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="13" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A13" s="4" t="str">
         <f t="shared" si="0"/>
         <v>0041500404</v>
@@ -4130,7 +4139,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="14" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A14" s="4" t="str">
         <f t="shared" si="0"/>
         <v>0041500404</v>
@@ -4243,7 +4252,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="15" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A15" s="4" t="str">
         <f t="shared" si="0"/>
         <v>0041500404</v>
@@ -4339,7 +4348,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="16" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A16" s="4" t="str">
         <f t="shared" si="0"/>
         <v>0041500404</v>
@@ -4450,7 +4459,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="17" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A17" s="4" t="str">
         <f t="shared" si="0"/>
         <v>0041500404</v>
@@ -4563,7 +4572,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="18" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A18" s="4" t="str">
         <f t="shared" si="0"/>
         <v>0041500404</v>
@@ -4676,7 +4685,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="19" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A19" s="4" t="str">
         <f t="shared" si="0"/>
         <v>0041500404</v>
@@ -4776,7 +4785,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="20" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A20" s="4" t="str">
         <f t="shared" si="0"/>
         <v>0041500404</v>
@@ -4880,7 +4889,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="21" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A21" s="4" t="str">
         <f t="shared" si="0"/>
         <v>0041500404</v>
@@ -4972,7 +4981,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="22" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A22" s="4" t="str">
         <f t="shared" si="0"/>
         <v>0041500404</v>
@@ -5076,7 +5085,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="23" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A23" s="4" t="str">
         <f t="shared" si="0"/>
         <v>0041500404</v>
@@ -5172,7 +5181,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="24" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A24" s="4" t="str">
         <f t="shared" si="0"/>
         <v>0041500404</v>
@@ -5272,7 +5281,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="25" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A25" s="4" t="str">
         <f t="shared" si="0"/>
         <v>0041500404</v>
@@ -5383,7 +5392,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="26" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A26" s="4" t="str">
         <f t="shared" si="0"/>
         <v>0041500404</v>
@@ -5479,7 +5488,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="27" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A27" s="4" t="str">
         <f t="shared" si="0"/>
         <v>0041500404</v>
@@ -5579,7 +5588,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="28" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A28" s="4" t="str">
         <f t="shared" si="0"/>
         <v>0041500404</v>
@@ -5690,7 +5699,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="29" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A29" s="4" t="str">
         <f t="shared" si="0"/>
         <v>0041500404</v>
@@ -5782,7 +5791,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="30" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A30" s="4" t="str">
         <f t="shared" si="0"/>
         <v>0041500404</v>
@@ -5893,7 +5902,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="31" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A31" s="4" t="str">
         <f t="shared" si="0"/>
         <v>0041500404</v>
@@ -5989,7 +5998,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="32" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A32" s="4" t="str">
         <f t="shared" si="0"/>
         <v>0041500404</v>
@@ -6100,7 +6109,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="33" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A33" s="4" t="str">
         <f t="shared" si="0"/>
         <v>0041500404</v>
@@ -6192,7 +6201,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="34" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A34" s="4" t="str">
         <f t="shared" si="0"/>
         <v>0041500404</v>
@@ -6303,7 +6312,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="35" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A35" s="4" t="str">
         <f t="shared" si="0"/>
         <v>0041500404</v>
@@ -6399,7 +6408,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="36" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A36" s="4" t="str">
         <f t="shared" si="0"/>
         <v>0041500404</v>
@@ -6499,7 +6508,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="37" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A37" s="4" t="str">
         <f t="shared" si="0"/>
         <v>0041500404</v>
@@ -6599,7 +6608,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="38" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A38" s="4" t="str">
         <f t="shared" si="0"/>
         <v>0041500404</v>
@@ -6710,7 +6719,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="39" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A39" s="4" t="str">
         <f t="shared" si="0"/>
         <v>0041500404</v>
@@ -6806,7 +6815,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="40" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A40" s="4" t="str">
         <f t="shared" si="0"/>
         <v>0041500404</v>
@@ -6919,7 +6928,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="41" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A41" s="4" t="str">
         <f t="shared" si="0"/>
         <v>0041500404</v>
@@ -7011,7 +7020,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="42" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A42" s="4" t="str">
         <f t="shared" si="0"/>
         <v>0041500404</v>
@@ -7124,7 +7133,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="43" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A43" s="4" t="str">
         <f t="shared" si="0"/>
         <v>0041500404</v>
@@ -7222,7 +7231,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="44" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A44" s="4" t="str">
         <f t="shared" si="0"/>
         <v>0041500404</v>
@@ -7335,7 +7344,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="45" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A45" s="4" t="str">
         <f t="shared" si="0"/>
         <v>0041500404</v>
@@ -7446,7 +7455,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="46" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A46" s="4" t="str">
         <f t="shared" si="0"/>
         <v>0041500404</v>
@@ -7542,7 +7551,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="47" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A47" s="4" t="str">
         <f t="shared" si="0"/>
         <v>0041500404</v>
@@ -7655,7 +7664,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="48" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A48" s="4" t="str">
         <f t="shared" si="0"/>
         <v>0041500404</v>
@@ -7755,7 +7764,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="49" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A49" s="4" t="str">
         <f t="shared" si="0"/>
         <v>0041500404</v>
@@ -7859,7 +7868,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="50" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A50" s="4" t="str">
         <f t="shared" si="0"/>
         <v>0041500404</v>
@@ -7955,7 +7964,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="51" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A51" s="4" t="str">
         <f t="shared" si="0"/>
         <v>0041500404</v>
@@ -8068,7 +8077,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="52" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A52" s="4" t="str">
         <f t="shared" si="0"/>
         <v>0041500404</v>
@@ -8179,7 +8188,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="53" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A53" s="4" t="str">
         <f t="shared" si="0"/>
         <v>0041500404</v>
@@ -8275,7 +8284,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="54" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A54" s="4" t="str">
         <f t="shared" si="0"/>
         <v>0041500404</v>
@@ -8375,7 +8384,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="55" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A55" s="4" t="str">
         <f t="shared" si="0"/>
         <v>0041500404</v>
@@ -8475,7 +8484,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="56" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A56" s="4" t="str">
         <f t="shared" si="0"/>
         <v>0041500404</v>
@@ -8588,7 +8597,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="57" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A57" s="4" t="str">
         <f t="shared" si="0"/>
         <v>0041500404</v>
@@ -8688,7 +8697,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="58" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A58" s="4" t="str">
         <f t="shared" si="0"/>
         <v>0041500404</v>
@@ -8788,7 +8797,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="59" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A59" s="4" t="str">
         <f t="shared" si="0"/>
         <v>0041500404</v>
@@ -8892,7 +8901,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="60" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A60" s="4" t="str">
         <f t="shared" si="0"/>
         <v>0041500404</v>
@@ -8992,7 +9001,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="61" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A61" s="4" t="str">
         <f t="shared" si="0"/>
         <v>0041500404</v>
@@ -9103,7 +9112,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="62" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A62" s="4" t="str">
         <f t="shared" si="0"/>
         <v>0041500404</v>
@@ -9199,7 +9208,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="63" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A63" s="4" t="str">
         <f t="shared" si="0"/>
         <v>0041500404</v>
@@ -9310,7 +9319,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="64" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A64" s="4" t="str">
         <f t="shared" si="0"/>
         <v>0041500404</v>
@@ -9406,7 +9415,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="65" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A65" s="4" t="str">
         <f t="shared" si="0"/>
         <v>0041500404</v>
@@ -9517,7 +9526,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="66" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A66" s="4" t="str">
         <f t="shared" si="0"/>
         <v>0041500404</v>
@@ -9628,7 +9637,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="67" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A67" s="4" t="str">
         <f t="shared" ref="A67:A130" si="1">"0041500404"</f>
         <v>0041500404</v>
@@ -9739,7 +9748,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="68" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A68" s="4" t="str">
         <f t="shared" si="1"/>
         <v>0041500404</v>
@@ -9835,7 +9844,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="69" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A69" s="4" t="str">
         <f t="shared" si="1"/>
         <v>0041500404</v>
@@ -9946,7 +9955,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="70" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A70" s="4" t="str">
         <f t="shared" si="1"/>
         <v>0041500404</v>
@@ -10046,7 +10055,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="71" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A71" s="4" t="str">
         <f t="shared" si="1"/>
         <v>0041500404</v>
@@ -10150,7 +10159,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="72" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A72" s="4" t="str">
         <f t="shared" si="1"/>
         <v>0041500404</v>
@@ -10250,7 +10259,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="73" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A73" s="4" t="str">
         <f t="shared" si="1"/>
         <v>0041500404</v>
@@ -10350,7 +10359,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="74" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A74" s="4" t="str">
         <f t="shared" si="1"/>
         <v>0041500404</v>
@@ -10454,7 +10463,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="75" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A75" s="4" t="str">
         <f t="shared" si="1"/>
         <v>0041500404</v>
@@ -10565,7 +10574,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="76" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A76" s="4" t="str">
         <f t="shared" si="1"/>
         <v>0041500404</v>
@@ -10661,7 +10670,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="77" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A77" s="4" t="str">
         <f t="shared" si="1"/>
         <v>0041500404</v>
@@ -10761,7 +10770,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="78" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A78" s="4" t="str">
         <f t="shared" si="1"/>
         <v>0041500404</v>
@@ -10853,7 +10862,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="79" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A79" s="4" t="str">
         <f t="shared" si="1"/>
         <v>0041500404</v>
@@ -10953,7 +10962,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="80" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A80" s="4" t="str">
         <f t="shared" si="1"/>
         <v>0041500404</v>
@@ -11053,7 +11062,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="81" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A81" s="4" t="str">
         <f t="shared" si="1"/>
         <v>0041500404</v>
@@ -11157,7 +11166,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="82" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A82" s="4" t="str">
         <f t="shared" si="1"/>
         <v>0041500404</v>
@@ -11261,7 +11270,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="83" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A83" s="4" t="str">
         <f t="shared" si="1"/>
         <v>0041500404</v>
@@ -11372,7 +11381,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="84" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A84" s="4" t="str">
         <f t="shared" si="1"/>
         <v>0041500404</v>
@@ -11468,7 +11477,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="85" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A85" s="4" t="str">
         <f t="shared" si="1"/>
         <v>0041500404</v>
@@ -11579,7 +11588,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="86" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A86" s="4" t="str">
         <f t="shared" si="1"/>
         <v>0041500404</v>
@@ -11690,7 +11699,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="87" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A87" s="4" t="str">
         <f t="shared" si="1"/>
         <v>0041500404</v>
@@ -11790,7 +11799,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="88" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A88" s="4" t="str">
         <f t="shared" si="1"/>
         <v>0041500404</v>
@@ -11894,7 +11903,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="89" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A89" s="4" t="str">
         <f t="shared" si="1"/>
         <v>0041500404</v>
@@ -11998,7 +12007,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="90" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A90" s="4" t="str">
         <f t="shared" si="1"/>
         <v>0041500404</v>
@@ -12111,7 +12120,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="91" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A91" s="4" t="str">
         <f t="shared" si="1"/>
         <v>0041500404</v>
@@ -12222,7 +12231,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="92" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A92" s="4" t="str">
         <f t="shared" si="1"/>
         <v>0041500404</v>
@@ -12318,7 +12327,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="93" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A93" s="4" t="str">
         <f t="shared" si="1"/>
         <v>0041500404</v>
@@ -12429,7 +12438,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="94" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A94" s="4" t="str">
         <f t="shared" si="1"/>
         <v>0041500404</v>
@@ -12521,7 +12530,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="95" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A95" s="4" t="str">
         <f t="shared" si="1"/>
         <v>0041500404</v>
@@ -12621,7 +12630,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="96" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A96" s="4" t="str">
         <f t="shared" si="1"/>
         <v>0041500404</v>
@@ -12725,7 +12734,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="97" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A97" s="4" t="str">
         <f t="shared" si="1"/>
         <v>0041500404</v>
@@ -12825,7 +12834,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="98" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A98" s="4" t="str">
         <f t="shared" si="1"/>
         <v>0041500404</v>
@@ -12925,7 +12934,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="99" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A99" s="4" t="str">
         <f t="shared" si="1"/>
         <v>0041500404</v>
@@ -13025,7 +13034,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="100" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A100" s="4" t="str">
         <f t="shared" si="1"/>
         <v>0041500404</v>
@@ -13125,7 +13134,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="101" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A101" s="4" t="str">
         <f t="shared" si="1"/>
         <v>0041500404</v>
@@ -13229,7 +13238,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="102" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A102" s="4" t="str">
         <f t="shared" si="1"/>
         <v>0041500404</v>
@@ -13340,7 +13349,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="103" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A103" s="4" t="str">
         <f t="shared" si="1"/>
         <v>0041500404</v>
@@ -13436,7 +13445,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="104" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A104" s="4" t="str">
         <f t="shared" si="1"/>
         <v>0041500404</v>
@@ -13547,7 +13556,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="105" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A105" s="4" t="str">
         <f t="shared" si="1"/>
         <v>0041500404</v>
@@ -13639,7 +13648,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="106" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A106" s="4" t="str">
         <f t="shared" si="1"/>
         <v>0041500404</v>
@@ -13729,7 +13738,7 @@
       <c r="AQ106" s="4"/>
       <c r="AR106" s="4"/>
     </row>
-    <row r="107" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A107" s="4" t="str">
         <f t="shared" si="1"/>
         <v>0041500404</v>
@@ -13819,7 +13828,7 @@
       <c r="AQ107" s="4"/>
       <c r="AR107" s="4"/>
     </row>
-    <row r="108" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A108" s="4" t="str">
         <f t="shared" si="1"/>
         <v>0041500404</v>
@@ -13917,7 +13926,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="109" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A109" s="4" t="str">
         <f t="shared" si="1"/>
         <v>0041500404</v>
@@ -14028,7 +14037,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="110" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A110" s="4" t="str">
         <f t="shared" si="1"/>
         <v>0041500404</v>
@@ -14124,7 +14133,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="111" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A111" s="4" t="str">
         <f t="shared" si="1"/>
         <v>0041500404</v>
@@ -14235,7 +14244,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="112" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A112" s="4" t="str">
         <f t="shared" si="1"/>
         <v>0041500404</v>
@@ -14331,7 +14340,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="113" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A113" s="4" t="str">
         <f t="shared" si="1"/>
         <v>0041500404</v>
@@ -14442,7 +14451,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="114" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A114" s="4" t="str">
         <f t="shared" si="1"/>
         <v>0041500404</v>
@@ -14538,7 +14547,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="115" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A115" s="4" t="str">
         <f t="shared" si="1"/>
         <v>0041500404</v>
@@ -14649,7 +14658,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="116" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A116" s="4" t="str">
         <f t="shared" si="1"/>
         <v>0041500404</v>
@@ -14745,7 +14754,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="117" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A117" s="4" t="str">
         <f t="shared" si="1"/>
         <v>0041500404</v>
@@ -14858,7 +14867,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="118" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A118" s="4" t="str">
         <f t="shared" si="1"/>
         <v>0041500404</v>
@@ -14971,7 +14980,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="119" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A119" s="4" t="str">
         <f t="shared" si="1"/>
         <v>0041500404</v>
@@ -15084,7 +15093,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="120" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A120" s="4" t="str">
         <f t="shared" si="1"/>
         <v>0041500404</v>
@@ -15180,7 +15189,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="121" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A121" s="4" t="str">
         <f t="shared" si="1"/>
         <v>0041500404</v>
@@ -15280,7 +15289,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="122" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A122" s="4" t="str">
         <f t="shared" si="1"/>
         <v>0041500404</v>
@@ -15391,7 +15400,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="123" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A123" s="4" t="str">
         <f t="shared" si="1"/>
         <v>0041500404</v>
@@ -15487,7 +15496,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="124" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A124" s="4" t="str">
         <f t="shared" si="1"/>
         <v>0041500404</v>
@@ -15598,7 +15607,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="125" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A125" s="4" t="str">
         <f t="shared" si="1"/>
         <v>0041500404</v>
@@ -15694,7 +15703,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="126" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A126" s="4" t="str">
         <f t="shared" si="1"/>
         <v>0041500404</v>
@@ -15794,7 +15803,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="127" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A127" s="4" t="str">
         <f t="shared" si="1"/>
         <v>0041500404</v>
@@ -15898,7 +15907,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="128" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A128" s="4" t="str">
         <f t="shared" si="1"/>
         <v>0041500404</v>
@@ -16002,7 +16011,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="129" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A129" s="4" t="str">
         <f t="shared" si="1"/>
         <v>0041500404</v>
@@ -16102,7 +16111,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="130" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A130" s="4" t="str">
         <f t="shared" si="1"/>
         <v>0041500404</v>
@@ -16213,7 +16222,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="131" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A131" s="4" t="str">
         <f t="shared" ref="A131:A194" si="2">"0041500404"</f>
         <v>0041500404</v>
@@ -16309,7 +16318,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="132" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A132" s="4" t="str">
         <f t="shared" si="2"/>
         <v>0041500404</v>
@@ -16420,7 +16429,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="133" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A133" s="4" t="str">
         <f t="shared" si="2"/>
         <v>0041500404</v>
@@ -16516,7 +16525,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="134" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A134" s="4" t="str">
         <f t="shared" si="2"/>
         <v>0041500404</v>
@@ -16629,7 +16638,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="135" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A135" s="4" t="str">
         <f t="shared" si="2"/>
         <v>0041500404</v>
@@ -16729,7 +16738,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="136" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A136" s="4" t="str">
         <f t="shared" si="2"/>
         <v>0041500404</v>
@@ -16819,7 +16828,7 @@
       <c r="AQ136" s="4"/>
       <c r="AR136" s="4"/>
     </row>
-    <row r="137" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A137" s="4" t="str">
         <f t="shared" si="2"/>
         <v>0041500404</v>
@@ -16919,7 +16928,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="138" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A138" s="4" t="str">
         <f t="shared" si="2"/>
         <v>0041500404</v>
@@ -17019,7 +17028,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="139" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A139" s="4" t="str">
         <f t="shared" si="2"/>
         <v>0041500404</v>
@@ -17119,7 +17128,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="140" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A140" s="4" t="str">
         <f t="shared" si="2"/>
         <v>0041500404</v>
@@ -17230,7 +17239,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="141" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A141" s="4" t="str">
         <f t="shared" si="2"/>
         <v>0041500404</v>
@@ -17326,7 +17335,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="142" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A142" s="4" t="str">
         <f t="shared" si="2"/>
         <v>0041500404</v>
@@ -17437,7 +17446,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="143" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A143" s="4" t="str">
         <f t="shared" si="2"/>
         <v>0041500404</v>
@@ -17533,7 +17542,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="144" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A144" s="4" t="str">
         <f t="shared" si="2"/>
         <v>0041500404</v>
@@ -17633,7 +17642,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="145" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A145" s="4" t="str">
         <f t="shared" si="2"/>
         <v>0041500404</v>
@@ -17737,7 +17746,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="146" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A146" s="4" t="str">
         <f t="shared" si="2"/>
         <v>0041500404</v>
@@ -17829,7 +17838,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="147" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A147" s="4" t="str">
         <f t="shared" si="2"/>
         <v>0041500404</v>
@@ -17929,7 +17938,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="148" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A148" s="4" t="str">
         <f t="shared" si="2"/>
         <v>0041500404</v>
@@ -18033,7 +18042,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="149" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A149" s="4" t="str">
         <f t="shared" si="2"/>
         <v>0041500404</v>
@@ -18144,7 +18153,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="150" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A150" s="4" t="str">
         <f t="shared" si="2"/>
         <v>0041500404</v>
@@ -18240,7 +18249,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="151" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A151" s="4" t="str">
         <f t="shared" si="2"/>
         <v>0041500404</v>
@@ -18336,7 +18345,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="152" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A152" s="4" t="str">
         <f t="shared" si="2"/>
         <v>0041500404</v>
@@ -18436,7 +18445,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="153" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A153" s="4" t="str">
         <f t="shared" si="2"/>
         <v>0041500404</v>
@@ -18547,7 +18556,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="154" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A154" s="4" t="str">
         <f t="shared" si="2"/>
         <v>0041500404</v>
@@ -18658,7 +18667,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="155" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A155" s="4" t="str">
         <f t="shared" si="2"/>
         <v>0041500404</v>
@@ -18756,7 +18765,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="156" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A156" s="4" t="str">
         <f t="shared" si="2"/>
         <v>0041500404</v>
@@ -18856,7 +18865,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="157" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A157" s="4" t="str">
         <f t="shared" si="2"/>
         <v>0041500404</v>
@@ -18960,7 +18969,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="158" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A158" s="4" t="str">
         <f t="shared" si="2"/>
         <v>0041500404</v>
@@ -19052,7 +19061,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="159" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A159" s="4" t="str">
         <f t="shared" si="2"/>
         <v>0041500404</v>
@@ -19156,7 +19165,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="160" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A160" s="4" t="str">
         <f t="shared" si="2"/>
         <v>0041500404</v>
@@ -19267,7 +19276,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="161" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A161" s="4" t="str">
         <f t="shared" si="2"/>
         <v>0041500404</v>
@@ -19363,7 +19372,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="162" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A162" s="4" t="str">
         <f t="shared" si="2"/>
         <v>0041500404</v>
@@ -19463,7 +19472,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="163" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A163" s="4" t="str">
         <f t="shared" si="2"/>
         <v>0041500404</v>
@@ -19567,7 +19576,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="164" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A164" s="4" t="str">
         <f t="shared" si="2"/>
         <v>0041500404</v>
@@ -19667,7 +19676,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="165" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A165" s="4" t="str">
         <f t="shared" si="2"/>
         <v>0041500404</v>
@@ -19767,7 +19776,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="166" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A166" s="4" t="str">
         <f t="shared" si="2"/>
         <v>0041500404</v>
@@ -19871,7 +19880,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="167" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A167" s="4" t="str">
         <f t="shared" si="2"/>
         <v>0041500404</v>
@@ -19982,7 +19991,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="168" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A168" s="4" t="str">
         <f t="shared" si="2"/>
         <v>0041500404</v>
@@ -20078,7 +20087,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="169" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A169" s="4" t="str">
         <f t="shared" si="2"/>
         <v>0041500404</v>
@@ -20189,7 +20198,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="170" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A170" s="4" t="str">
         <f t="shared" si="2"/>
         <v>0041500404</v>
@@ -20285,7 +20294,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="171" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A171" s="4" t="str">
         <f t="shared" si="2"/>
         <v>0041500404</v>
@@ -20396,7 +20405,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="172" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A172" s="4" t="str">
         <f t="shared" si="2"/>
         <v>0041500404</v>
@@ -20488,7 +20497,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="173" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A173" s="4" t="str">
         <f t="shared" si="2"/>
         <v>0041500404</v>
@@ -20588,7 +20597,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="174" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A174" s="4" t="str">
         <f t="shared" si="2"/>
         <v>0041500404</v>
@@ -20680,7 +20689,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="175" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A175" s="4" t="str">
         <f t="shared" si="2"/>
         <v>0041500404</v>
@@ -20780,7 +20789,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="176" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A176" s="4" t="str">
         <f t="shared" si="2"/>
         <v>0041500404</v>
@@ -20880,7 +20889,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="177" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A177" s="4" t="str">
         <f t="shared" si="2"/>
         <v>0041500404</v>
@@ -20984,7 +20993,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="178" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A178" s="4" t="str">
         <f t="shared" si="2"/>
         <v>0041500404</v>
@@ -21076,7 +21085,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="179" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A179" s="4" t="str">
         <f t="shared" si="2"/>
         <v>0041500404</v>
@@ -21180,7 +21189,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="180" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A180" s="4" t="str">
         <f t="shared" si="2"/>
         <v>0041500404</v>
@@ -21276,7 +21285,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="181" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A181" s="4" t="str">
         <f t="shared" si="2"/>
         <v>0041500404</v>
@@ -21376,7 +21385,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="182" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A182" s="4" t="str">
         <f t="shared" si="2"/>
         <v>0041500404</v>
@@ -21480,7 +21489,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="183" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A183" s="4" t="str">
         <f t="shared" si="2"/>
         <v>0041500404</v>
@@ -21572,7 +21581,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="184" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A184" s="4" t="str">
         <f t="shared" si="2"/>
         <v>0041500404</v>
@@ -21672,7 +21681,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="185" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A185" s="4" t="str">
         <f t="shared" si="2"/>
         <v>0041500404</v>
@@ -21776,7 +21785,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="186" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A186" s="4" t="str">
         <f t="shared" si="2"/>
         <v>0041500404</v>
@@ -21872,7 +21881,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="187" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A187" s="4" t="str">
         <f t="shared" si="2"/>
         <v>0041500404</v>
@@ -21985,7 +21994,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="188" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A188" s="4" t="str">
         <f t="shared" si="2"/>
         <v>0041500404</v>
@@ -22098,7 +22107,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="189" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A189" s="4" t="str">
         <f t="shared" si="2"/>
         <v>0041500404</v>
@@ -22190,7 +22199,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="190" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A190" s="4" t="str">
         <f t="shared" si="2"/>
         <v>0041500404</v>
@@ -22290,7 +22299,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="191" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A191" s="4" t="str">
         <f t="shared" si="2"/>
         <v>0041500404</v>
@@ -22388,7 +22397,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="192" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A192" s="4" t="str">
         <f t="shared" si="2"/>
         <v>0041500404</v>
@@ -22492,7 +22501,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="193" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A193" s="4" t="str">
         <f t="shared" si="2"/>
         <v>0041500404</v>
@@ -22592,7 +22601,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="194" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A194" s="4" t="str">
         <f t="shared" si="2"/>
         <v>0041500404</v>
@@ -22692,7 +22701,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="195" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A195" s="4" t="str">
         <f t="shared" ref="A195:A258" si="3">"0041500404"</f>
         <v>0041500404</v>
@@ -22803,7 +22812,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="196" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A196" s="4" t="str">
         <f t="shared" si="3"/>
         <v>0041500404</v>
@@ -22899,7 +22908,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="197" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A197" s="4" t="str">
         <f t="shared" si="3"/>
         <v>0041500404</v>
@@ -23010,7 +23019,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="198" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A198" s="4" t="str">
         <f t="shared" si="3"/>
         <v>0041500404</v>
@@ -23121,7 +23130,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="199" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A199" s="4" t="str">
         <f t="shared" si="3"/>
         <v>0041500404</v>
@@ -23234,7 +23243,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="200" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A200" s="4" t="str">
         <f t="shared" si="3"/>
         <v>0041500404</v>
@@ -23326,7 +23335,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="201" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A201" s="4" t="str">
         <f t="shared" si="3"/>
         <v>0041500404</v>
@@ -23418,7 +23427,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="202" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A202" s="4" t="str">
         <f t="shared" si="3"/>
         <v>0041500404</v>
@@ -23518,7 +23527,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="203" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A203" s="4" t="str">
         <f t="shared" si="3"/>
         <v>0041500404</v>
@@ -23629,7 +23638,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="204" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A204" s="4" t="str">
         <f t="shared" si="3"/>
         <v>0041500404</v>
@@ -23729,7 +23738,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="205" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A205" s="4" t="str">
         <f t="shared" si="3"/>
         <v>0041500404</v>
@@ -23833,7 +23842,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="206" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A206" s="4" t="str">
         <f t="shared" si="3"/>
         <v>0041500404</v>
@@ -23937,7 +23946,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="207" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A207" s="4" t="str">
         <f t="shared" si="3"/>
         <v>0041500404</v>
@@ -24033,7 +24042,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="208" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A208" s="4" t="str">
         <f t="shared" si="3"/>
         <v>0041500404</v>
@@ -24144,7 +24153,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="209" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A209" s="4" t="str">
         <f t="shared" si="3"/>
         <v>0041500404</v>
@@ -24240,7 +24249,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="210" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A210" s="4" t="str">
         <f t="shared" si="3"/>
         <v>0041500404</v>
@@ -24353,7 +24362,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="211" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A211" s="4" t="str">
         <f t="shared" si="3"/>
         <v>0041500404</v>
@@ -24466,7 +24475,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="212" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A212" s="4" t="str">
         <f t="shared" si="3"/>
         <v>0041500404</v>
@@ -24577,7 +24586,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="213" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A213" s="4" t="str">
         <f t="shared" si="3"/>
         <v>0041500404</v>
@@ -24669,7 +24678,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="214" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A214" s="4" t="str">
         <f t="shared" si="3"/>
         <v>0041500404</v>
@@ -24780,7 +24789,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="215" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A215" s="4" t="str">
         <f t="shared" si="3"/>
         <v>0041500404</v>
@@ -24872,7 +24881,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="216" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A216" s="4" t="str">
         <f t="shared" si="3"/>
         <v>0041500404</v>
@@ -24972,7 +24981,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="217" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A217" s="4" t="str">
         <f t="shared" si="3"/>
         <v>0041500404</v>
@@ -25083,7 +25092,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="218" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A218" s="4" t="str">
         <f t="shared" si="3"/>
         <v>0041500404</v>
@@ -25183,7 +25192,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="219" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A219" s="4" t="str">
         <f t="shared" si="3"/>
         <v>0041500404</v>
@@ -25287,7 +25296,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="220" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A220" s="4" t="str">
         <f t="shared" si="3"/>
         <v>0041500404</v>
@@ -25398,7 +25407,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="221" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A221" s="4" t="str">
         <f t="shared" si="3"/>
         <v>0041500404</v>
@@ -25498,7 +25507,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="222" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A222" s="4" t="str">
         <f t="shared" si="3"/>
         <v>0041500404</v>
@@ -25611,7 +25620,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="223" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A223" s="4" t="str">
         <f t="shared" si="3"/>
         <v>0041500404</v>
@@ -25722,7 +25731,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="224" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A224" s="4" t="str">
         <f t="shared" si="3"/>
         <v>0041500404</v>
@@ -25818,7 +25827,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="225" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A225" s="4" t="str">
         <f t="shared" si="3"/>
         <v>0041500404</v>
@@ -25914,7 +25923,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="226" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="226" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A226" s="4" t="str">
         <f t="shared" si="3"/>
         <v>0041500404</v>
@@ -26025,7 +26034,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="227" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A227" s="4" t="str">
         <f t="shared" si="3"/>
         <v>0041500404</v>
@@ -26123,7 +26132,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="228" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="228" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A228" s="4" t="str">
         <f t="shared" si="3"/>
         <v>0041500404</v>
@@ -26234,7 +26243,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="229" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A229" s="4" t="str">
         <f t="shared" si="3"/>
         <v>0041500404</v>
@@ -26345,7 +26354,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="230" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="230" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A230" s="4" t="str">
         <f t="shared" si="3"/>
         <v>0041500404</v>
@@ -26456,7 +26465,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="231" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="231" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A231" s="4" t="str">
         <f t="shared" si="3"/>
         <v>0041500404</v>
@@ -26552,7 +26561,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="232" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="232" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A232" s="4" t="str">
         <f t="shared" si="3"/>
         <v>0041500404</v>
@@ -26663,7 +26672,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="233" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="233" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A233" s="4" t="str">
         <f t="shared" si="3"/>
         <v>0041500404</v>
@@ -26755,7 +26764,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="234" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="234" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A234" s="4" t="str">
         <f t="shared" si="3"/>
         <v>0041500404</v>
@@ -26845,7 +26854,7 @@
       <c r="AQ234" s="4"/>
       <c r="AR234" s="4"/>
     </row>
-    <row r="235" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="235" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A235" s="4" t="str">
         <f t="shared" si="3"/>
         <v>0041500404</v>
@@ -26935,7 +26944,7 @@
       <c r="AQ235" s="4"/>
       <c r="AR235" s="4"/>
     </row>
-    <row r="236" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="236" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A236" s="4" t="str">
         <f t="shared" si="3"/>
         <v>0041500404</v>
@@ -27027,7 +27036,7 @@
       <c r="AQ236" s="4"/>
       <c r="AR236" s="4"/>
     </row>
-    <row r="237" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="237" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A237" s="4" t="str">
         <f t="shared" si="3"/>
         <v>0041500404</v>
@@ -27131,7 +27140,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="238" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="238" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A238" s="4" t="str">
         <f t="shared" si="3"/>
         <v>0041500404</v>
@@ -27244,7 +27253,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="239" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="239" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A239" s="4" t="str">
         <f t="shared" si="3"/>
         <v>0041500404</v>
@@ -27355,7 +27364,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="240" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="240" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A240" s="4" t="str">
         <f t="shared" si="3"/>
         <v>0041500404</v>
@@ -27451,7 +27460,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="241" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="241" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A241" s="4" t="str">
         <f t="shared" si="3"/>
         <v>0041500404</v>
@@ -27562,7 +27571,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="242" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="242" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A242" s="4" t="str">
         <f t="shared" si="3"/>
         <v>0041500404</v>
@@ -27654,7 +27663,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="243" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="243" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A243" s="4" t="str">
         <f t="shared" si="3"/>
         <v>0041500404</v>
@@ -27754,7 +27763,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="244" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="244" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A244" s="4" t="str">
         <f t="shared" si="3"/>
         <v>0041500404</v>
@@ -27867,7 +27876,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="245" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="245" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A245" s="4" t="str">
         <f t="shared" si="3"/>
         <v>0041500404</v>
@@ -27978,7 +27987,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="246" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="246" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A246" s="4" t="str">
         <f t="shared" si="3"/>
         <v>0041500404</v>
@@ -28074,7 +28083,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="247" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="247" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A247" s="4" t="str">
         <f t="shared" si="3"/>
         <v>0041500404</v>
@@ -28187,7 +28196,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="248" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="248" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A248" s="4" t="str">
         <f t="shared" si="3"/>
         <v>0041500404</v>
@@ -28283,7 +28292,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="249" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="249" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A249" s="4" t="str">
         <f t="shared" si="3"/>
         <v>0041500404</v>
@@ -28383,7 +28392,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="250" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="250" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A250" s="4" t="str">
         <f t="shared" si="3"/>
         <v>0041500404</v>
@@ -28483,7 +28492,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="251" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="251" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A251" s="4" t="str">
         <f t="shared" si="3"/>
         <v>0041500404</v>
@@ -28594,7 +28603,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="252" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="252" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A252" s="4" t="str">
         <f t="shared" si="3"/>
         <v>0041500404</v>
@@ -28690,7 +28699,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="253" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="253" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A253" s="4" t="str">
         <f t="shared" si="3"/>
         <v>0041500404</v>
@@ -28801,7 +28810,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="254" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="254" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A254" s="4" t="str">
         <f t="shared" si="3"/>
         <v>0041500404</v>
@@ -28897,7 +28906,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="255" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="255" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A255" s="4" t="str">
         <f t="shared" si="3"/>
         <v>0041500404</v>
@@ -29008,7 +29017,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="256" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="256" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A256" s="4" t="str">
         <f t="shared" si="3"/>
         <v>0041500404</v>
@@ -29108,7 +29117,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="257" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="257" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A257" s="4" t="str">
         <f t="shared" si="3"/>
         <v>0041500404</v>
@@ -29212,7 +29221,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="258" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="258" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A258" s="4" t="str">
         <f t="shared" si="3"/>
         <v>0041500404</v>
@@ -29316,7 +29325,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="259" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="259" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A259" s="4" t="str">
         <f t="shared" ref="A259:A322" si="4">"0041500404"</f>
         <v>0041500404</v>
@@ -29416,7 +29425,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="260" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="260" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A260" s="4" t="str">
         <f t="shared" si="4"/>
         <v>0041500404</v>
@@ -29527,7 +29536,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="261" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="261" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A261" s="4" t="str">
         <f t="shared" si="4"/>
         <v>0041500404</v>
@@ -29640,7 +29649,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="262" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="262" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A262" s="4" t="str">
         <f t="shared" si="4"/>
         <v>0041500404</v>
@@ -29753,7 +29762,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="263" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="263" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A263" s="4" t="str">
         <f t="shared" si="4"/>
         <v>0041500404</v>
@@ -29849,7 +29858,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="264" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="264" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A264" s="4" t="str">
         <f t="shared" si="4"/>
         <v>0041500404</v>
@@ -29962,7 +29971,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="265" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="265" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A265" s="4" t="str">
         <f t="shared" si="4"/>
         <v>0041500404</v>
@@ -30054,7 +30063,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="266" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="266" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A266" s="4" t="str">
         <f t="shared" si="4"/>
         <v>0041500404</v>
@@ -30154,7 +30163,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="267" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="267" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A267" s="4" t="str">
         <f t="shared" si="4"/>
         <v>0041500404</v>
@@ -30267,7 +30276,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="268" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="268" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A268" s="4" t="str">
         <f t="shared" si="4"/>
         <v>0041500404</v>
@@ -30380,7 +30389,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="269" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="269" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A269" s="4" t="str">
         <f t="shared" si="4"/>
         <v>0041500404</v>
@@ -30491,7 +30500,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="270" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="270" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A270" s="4" t="str">
         <f t="shared" si="4"/>
         <v>0041500404</v>
@@ -30602,7 +30611,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="271" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="271" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A271" s="4" t="str">
         <f t="shared" si="4"/>
         <v>0041500404</v>
@@ -30698,7 +30707,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="272" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="272" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A272" s="4" t="str">
         <f t="shared" si="4"/>
         <v>0041500404</v>
@@ -30809,7 +30818,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="273" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="273" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A273" s="4" t="str">
         <f t="shared" si="4"/>
         <v>0041500404</v>
@@ -30905,7 +30914,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="274" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="274" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A274" s="4" t="str">
         <f t="shared" si="4"/>
         <v>0041500404</v>
@@ -31018,7 +31027,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="275" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="275" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A275" s="4" t="str">
         <f t="shared" si="4"/>
         <v>0041500404</v>
@@ -31118,7 +31127,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="276" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="276" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A276" s="4" t="str">
         <f t="shared" si="4"/>
         <v>0041500404</v>
@@ -31218,7 +31227,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="277" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="277" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A277" s="4" t="str">
         <f t="shared" si="4"/>
         <v>0041500404</v>
@@ -31312,7 +31321,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="278" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="278" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A278" s="4" t="str">
         <f t="shared" si="4"/>
         <v>0041500404</v>
@@ -31423,7 +31432,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="279" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="279" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A279" s="4" t="str">
         <f t="shared" si="4"/>
         <v>0041500404</v>
@@ -31519,7 +31528,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="280" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="280" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A280" s="4" t="str">
         <f t="shared" si="4"/>
         <v>0041500404</v>
@@ -31630,7 +31639,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="281" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="281" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A281" s="4" t="str">
         <f t="shared" si="4"/>
         <v>0041500404</v>
@@ -31726,7 +31735,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="282" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="282" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A282" s="4" t="str">
         <f t="shared" si="4"/>
         <v>0041500404</v>
@@ -31839,7 +31848,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="283" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="283" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A283" s="4" t="str">
         <f t="shared" si="4"/>
         <v>0041500404</v>
@@ -31937,7 +31946,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="284" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="284" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A284" s="4" t="str">
         <f t="shared" si="4"/>
         <v>0041500404</v>
@@ -32048,7 +32057,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="285" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="285" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A285" s="4" t="str">
         <f t="shared" si="4"/>
         <v>0041500404</v>
@@ -32144,7 +32153,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="286" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="286" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A286" s="4" t="str">
         <f t="shared" si="4"/>
         <v>0041500404</v>
@@ -32244,7 +32253,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="287" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="287" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A287" s="4" t="str">
         <f t="shared" si="4"/>
         <v>0041500404</v>
@@ -32344,7 +32353,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="288" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="288" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A288" s="4" t="str">
         <f t="shared" si="4"/>
         <v>0041500404</v>
@@ -32457,7 +32466,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="289" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="289" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A289" s="4" t="str">
         <f t="shared" si="4"/>
         <v>0041500404</v>
@@ -32568,7 +32577,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="290" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="290" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A290" s="4" t="str">
         <f t="shared" si="4"/>
         <v>0041500404</v>
@@ -32664,7 +32673,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="291" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="291" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A291" s="4" t="str">
         <f t="shared" si="4"/>
         <v>0041500404</v>
@@ -32777,7 +32786,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="292" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="292" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A292" s="4" t="str">
         <f t="shared" si="4"/>
         <v>0041500404</v>
@@ -32869,7 +32878,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="293" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="293" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A293" s="4" t="str">
         <f t="shared" si="4"/>
         <v>0041500404</v>
@@ -32969,7 +32978,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="294" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="294" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A294" s="4" t="str">
         <f t="shared" si="4"/>
         <v>0041500404</v>
@@ -33069,7 +33078,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="295" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="295" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A295" s="4" t="str">
         <f t="shared" si="4"/>
         <v>0041500404</v>
@@ -33169,7 +33178,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="296" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="296" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A296" s="4" t="str">
         <f t="shared" si="4"/>
         <v>0041500404</v>
@@ -33269,7 +33278,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="297" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="297" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A297" s="4" t="str">
         <f t="shared" si="4"/>
         <v>0041500404</v>
@@ -33369,7 +33378,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="298" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="298" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A298" s="4" t="str">
         <f t="shared" si="4"/>
         <v>0041500404</v>
@@ -33459,7 +33468,7 @@
       <c r="AQ298" s="4"/>
       <c r="AR298" s="4"/>
     </row>
-    <row r="299" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="299" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A299" s="4" t="str">
         <f t="shared" si="4"/>
         <v>0041500404</v>
@@ -33563,7 +33572,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="300" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="300" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A300" s="4" t="str">
         <f t="shared" si="4"/>
         <v>0041500404</v>
@@ -33655,7 +33664,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="301" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="301" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A301" s="4" t="str">
         <f t="shared" si="4"/>
         <v>0041500404</v>
@@ -33759,7 +33768,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="302" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="302" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A302" s="4" t="str">
         <f t="shared" si="4"/>
         <v>0041500404</v>
@@ -33855,7 +33864,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="303" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="303" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A303" s="4" t="str">
         <f t="shared" si="4"/>
         <v>0041500404</v>
@@ -33966,7 +33975,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="304" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="304" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A304" s="4" t="str">
         <f t="shared" si="4"/>
         <v>0041500404</v>
@@ -34062,7 +34071,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="305" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="305" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A305" s="4" t="str">
         <f t="shared" si="4"/>
         <v>0041500404</v>
@@ -34173,7 +34182,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="306" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="306" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A306" s="4" t="str">
         <f t="shared" si="4"/>
         <v>0041500404</v>
@@ -34273,7 +34282,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="307" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="307" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A307" s="4" t="str">
         <f t="shared" si="4"/>
         <v>0041500404</v>
@@ -34363,7 +34372,7 @@
       <c r="AQ307" s="4"/>
       <c r="AR307" s="4"/>
     </row>
-    <row r="308" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="308" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A308" s="4" t="str">
         <f t="shared" si="4"/>
         <v>0041500404</v>
@@ -34467,7 +34476,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="309" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="309" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A309" s="4" t="str">
         <f t="shared" si="4"/>
         <v>0041500404</v>
@@ -34571,7 +34580,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="310" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="310" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A310" s="4" t="str">
         <f t="shared" si="4"/>
         <v>0041500404</v>
@@ -34682,7 +34691,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="311" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="311" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A311" s="4" t="str">
         <f t="shared" si="4"/>
         <v>0041500404</v>
@@ -34778,7 +34787,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="312" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="312" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A312" s="4" t="str">
         <f t="shared" si="4"/>
         <v>0041500404</v>
@@ -34889,7 +34898,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="313" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="313" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A313" s="4" t="str">
         <f t="shared" si="4"/>
         <v>0041500404</v>
@@ -35002,7 +35011,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="314" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="314" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A314" s="4" t="str">
         <f t="shared" si="4"/>
         <v>0041500404</v>
@@ -35094,7 +35103,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="315" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="315" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A315" s="4" t="str">
         <f t="shared" si="4"/>
         <v>0041500404</v>
@@ -35186,7 +35195,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="316" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="316" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A316" s="4" t="str">
         <f t="shared" si="4"/>
         <v>0041500404</v>
@@ -35299,7 +35308,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="317" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="317" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A317" s="4" t="str">
         <f t="shared" si="4"/>
         <v>0041500404</v>
@@ -35391,7 +35400,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="318" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="318" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A318" s="4" t="str">
         <f t="shared" si="4"/>
         <v>0041500404</v>
@@ -35502,7 +35511,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="319" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="319" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A319" s="4" t="str">
         <f t="shared" si="4"/>
         <v>0041500404</v>
@@ -35598,7 +35607,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="320" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="320" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A320" s="4" t="str">
         <f t="shared" si="4"/>
         <v>0041500404</v>
@@ -35709,7 +35718,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="321" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="321" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A321" s="4" t="str">
         <f t="shared" si="4"/>
         <v>0041500404</v>
@@ -35805,7 +35814,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="322" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="322" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A322" s="4" t="str">
         <f t="shared" si="4"/>
         <v>0041500404</v>
@@ -35916,7 +35925,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="323" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="323" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A323" s="4" t="str">
         <f t="shared" ref="A323:A386" si="5">"0041500404"</f>
         <v>0041500404</v>
@@ -36008,7 +36017,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="324" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="324" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A324" s="4" t="str">
         <f t="shared" si="5"/>
         <v>0041500404</v>
@@ -36121,7 +36130,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="325" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="325" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A325" s="4" t="str">
         <f t="shared" si="5"/>
         <v>0041500404</v>
@@ -36232,7 +36241,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="326" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="326" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A326" s="4" t="str">
         <f t="shared" si="5"/>
         <v>0041500404</v>
@@ -36328,7 +36337,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="327" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="327" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A327" s="4" t="str">
         <f t="shared" si="5"/>
         <v>0041500404</v>
@@ -36428,7 +36437,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="328" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="328" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A328" s="4" t="str">
         <f t="shared" si="5"/>
         <v>0041500404</v>
@@ -36532,7 +36541,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="329" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="329" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A329" s="4" t="str">
         <f t="shared" si="5"/>
         <v>0041500404</v>
@@ -36636,7 +36645,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="330" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="330" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A330" s="4" t="str">
         <f t="shared" si="5"/>
         <v>0041500404</v>
@@ -36732,7 +36741,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="331" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="331" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A331" s="4" t="str">
         <f t="shared" si="5"/>
         <v>0041500404</v>
@@ -36845,7 +36854,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="332" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="332" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A332" s="4" t="str">
         <f t="shared" si="5"/>
         <v>0041500404</v>
@@ -36956,7 +36965,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="333" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="333" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A333" s="4" t="str">
         <f t="shared" si="5"/>
         <v>0041500404</v>
@@ -37067,7 +37076,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="334" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="334" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A334" s="4" t="str">
         <f t="shared" si="5"/>
         <v>0041500404</v>
@@ -37163,7 +37172,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="335" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="335" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A335" s="4" t="str">
         <f t="shared" si="5"/>
         <v>0041500404</v>
@@ -37263,7 +37272,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="336" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="336" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A336" s="4" t="str">
         <f t="shared" si="5"/>
         <v>0041500404</v>
@@ -37367,7 +37376,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="337" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="337" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A337" s="4" t="str">
         <f t="shared" si="5"/>
         <v>0041500404</v>
@@ -37467,7 +37476,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="338" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="338" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A338" s="4" t="str">
         <f t="shared" si="5"/>
         <v>0041500404</v>
@@ -37567,7 +37576,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="339" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="339" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A339" s="4" t="str">
         <f t="shared" si="5"/>
         <v>0041500404</v>
@@ -37667,7 +37676,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="340" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="340" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A340" s="4" t="str">
         <f t="shared" si="5"/>
         <v>0041500404</v>
@@ -37767,7 +37776,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="341" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="341" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A341" s="4" t="str">
         <f t="shared" si="5"/>
         <v>0041500404</v>
@@ -37871,7 +37880,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="342" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="342" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A342" s="4" t="str">
         <f t="shared" si="5"/>
         <v>0041500404</v>
@@ -37982,7 +37991,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="343" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="343" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A343" s="4" t="str">
         <f t="shared" si="5"/>
         <v>0041500404</v>
@@ -38074,7 +38083,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="344" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="344" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A344" s="4" t="str">
         <f t="shared" si="5"/>
         <v>0041500404</v>
@@ -38164,7 +38173,7 @@
       <c r="AQ344" s="4"/>
       <c r="AR344" s="4"/>
     </row>
-    <row r="345" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="345" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A345" s="4" t="str">
         <f t="shared" si="5"/>
         <v>0041500404</v>
@@ -38254,7 +38263,7 @@
       <c r="AQ345" s="4"/>
       <c r="AR345" s="4"/>
     </row>
-    <row r="346" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="346" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A346" s="4" t="str">
         <f t="shared" si="5"/>
         <v>0041500404</v>
@@ -38352,7 +38361,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="347" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="347" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A347" s="4" t="str">
         <f t="shared" si="5"/>
         <v>0041500404</v>
@@ -38465,7 +38474,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="348" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="348" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A348" s="4" t="str">
         <f t="shared" si="5"/>
         <v>0041500404</v>
@@ -38576,7 +38585,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="349" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="349" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A349" s="4" t="str">
         <f t="shared" si="5"/>
         <v>0041500404</v>
@@ -38672,7 +38681,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="350" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="350" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A350" s="4" t="str">
         <f t="shared" si="5"/>
         <v>0041500404</v>
@@ -38783,7 +38792,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="351" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="351" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A351" s="4" t="str">
         <f t="shared" si="5"/>
         <v>0041500404</v>
@@ -38896,7 +38905,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="352" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="352" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A352" s="4" t="str">
         <f t="shared" si="5"/>
         <v>0041500404</v>
@@ -39007,7 +39016,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="353" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="353" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A353" s="4" t="str">
         <f t="shared" si="5"/>
         <v>0041500404</v>
@@ -39103,7 +39112,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="354" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="354" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A354" s="4" t="str">
         <f t="shared" si="5"/>
         <v>0041500404</v>
@@ -39214,7 +39223,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="355" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="355" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A355" s="4" t="str">
         <f t="shared" si="5"/>
         <v>0041500404</v>
@@ -39327,7 +39336,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="356" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="356" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A356" s="4" t="str">
         <f t="shared" si="5"/>
         <v>0041500404</v>
@@ -39440,7 +39449,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="357" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="357" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A357" s="4" t="str">
         <f t="shared" si="5"/>
         <v>0041500404</v>
@@ -39536,7 +39545,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="358" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="358" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A358" s="4" t="str">
         <f t="shared" si="5"/>
         <v>0041500404</v>
@@ -39636,7 +39645,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="359" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="359" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A359" s="4" t="str">
         <f t="shared" si="5"/>
         <v>0041500404</v>
@@ -39747,7 +39756,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="360" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="360" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A360" s="4" t="str">
         <f t="shared" si="5"/>
         <v>0041500404</v>
@@ -39843,7 +39852,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="361" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="361" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A361" s="4" t="str">
         <f t="shared" si="5"/>
         <v>0041500404</v>
@@ -39943,7 +39952,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="362" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="362" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A362" s="4" t="str">
         <f t="shared" si="5"/>
         <v>0041500404</v>
@@ -40054,7 +40063,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="363" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="363" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A363" s="4" t="str">
         <f t="shared" si="5"/>
         <v>0041500404</v>
@@ -40146,7 +40155,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="364" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="364" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A364" s="4" t="str">
         <f t="shared" si="5"/>
         <v>0041500404</v>
@@ -40246,7 +40255,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="365" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="365" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A365" s="4" t="str">
         <f t="shared" si="5"/>
         <v>0041500404</v>
@@ -40346,7 +40355,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="366" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="366" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A366" s="4" t="str">
         <f t="shared" si="5"/>
         <v>0041500404</v>
@@ -40446,7 +40455,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="367" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="367" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A367" s="4" t="str">
         <f t="shared" si="5"/>
         <v>0041500404</v>
@@ -40550,7 +40559,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="368" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="368" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A368" s="4" t="str">
         <f t="shared" si="5"/>
         <v>0041500404</v>
@@ -40642,7 +40651,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="369" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="369" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A369" s="4" t="str">
         <f t="shared" si="5"/>
         <v>0041500404</v>
@@ -40746,7 +40755,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="370" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="370" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A370" s="4" t="str">
         <f t="shared" si="5"/>
         <v>0041500404</v>
@@ -40842,7 +40851,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="371" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="371" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A371" s="4" t="str">
         <f t="shared" si="5"/>
         <v>0041500404</v>
@@ -40953,7 +40962,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="372" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="372" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A372" s="4" t="str">
         <f t="shared" si="5"/>
         <v>0041500404</v>
@@ -41064,7 +41073,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="373" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="373" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A373" s="4" t="str">
         <f t="shared" si="5"/>
         <v>0041500404</v>
@@ -41160,7 +41169,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="374" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="374" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A374" s="4" t="str">
         <f t="shared" si="5"/>
         <v>0041500404</v>
@@ -41260,7 +41269,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="375" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="375" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A375" s="4" t="str">
         <f t="shared" si="5"/>
         <v>0041500404</v>
@@ -41371,7 +41380,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="376" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="376" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A376" s="4" t="str">
         <f t="shared" si="5"/>
         <v>0041500404</v>
@@ -41467,7 +41476,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="377" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="377" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A377" s="4" t="str">
         <f t="shared" si="5"/>
         <v>0041500404</v>
@@ -41567,7 +41576,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="378" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="378" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A378" s="4" t="str">
         <f t="shared" si="5"/>
         <v>0041500404</v>
@@ -41671,7 +41680,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="379" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="379" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A379" s="4" t="str">
         <f t="shared" si="5"/>
         <v>0041500404</v>
@@ -41771,7 +41780,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="380" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="380" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A380" s="4" t="str">
         <f t="shared" si="5"/>
         <v>0041500404</v>
@@ -41875,7 +41884,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="381" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="381" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A381" s="4" t="str">
         <f t="shared" si="5"/>
         <v>0041500404</v>
@@ -41971,7 +41980,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="382" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="382" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A382" s="4" t="str">
         <f t="shared" si="5"/>
         <v>0041500404</v>
@@ -42082,7 +42091,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="383" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="383" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A383" s="4" t="str">
         <f t="shared" si="5"/>
         <v>0041500404</v>
@@ -42178,7 +42187,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="384" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="384" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A384" s="4" t="str">
         <f t="shared" si="5"/>
         <v>0041500404</v>
@@ -42289,7 +42298,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="385" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="385" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A385" s="4" t="str">
         <f t="shared" si="5"/>
         <v>0041500404</v>
@@ -42385,7 +42394,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="386" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="386" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A386" s="4" t="str">
         <f t="shared" si="5"/>
         <v>0041500404</v>
@@ -42496,7 +42505,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="387" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="387" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A387" s="4" t="str">
         <f t="shared" ref="A387:A450" si="6">"0041500404"</f>
         <v>0041500404</v>
@@ -42607,7 +42616,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="388" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="388" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A388" s="4" t="str">
         <f t="shared" si="6"/>
         <v>0041500404</v>
@@ -42703,7 +42712,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="389" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="389" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A389" s="4" t="str">
         <f t="shared" si="6"/>
         <v>0041500404</v>
@@ -42814,7 +42823,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="390" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="390" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A390" s="4" t="str">
         <f t="shared" si="6"/>
         <v>0041500404</v>
@@ -42910,7 +42919,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="391" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="391" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A391" s="4" t="str">
         <f t="shared" si="6"/>
         <v>0041500404</v>
@@ -43021,7 +43030,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="392" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="392" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A392" s="4" t="str">
         <f t="shared" si="6"/>
         <v>0041500404</v>
@@ -43117,7 +43126,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="393" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="393" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A393" s="4" t="str">
         <f t="shared" si="6"/>
         <v>0041500404</v>
@@ -43228,7 +43237,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="394" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="394" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A394" s="4" t="str">
         <f t="shared" si="6"/>
         <v>0041500404</v>
@@ -43324,7 +43333,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="395" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="395" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A395" s="4" t="str">
         <f t="shared" si="6"/>
         <v>0041500404</v>
@@ -43437,7 +43446,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="396" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="396" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A396" s="4" t="str">
         <f t="shared" si="6"/>
         <v>0041500404</v>
@@ -43529,7 +43538,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="397" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="397" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A397" s="4" t="str">
         <f t="shared" si="6"/>
         <v>0041500404</v>
@@ -43619,7 +43628,7 @@
       <c r="AQ397" s="4"/>
       <c r="AR397" s="4"/>
     </row>
-    <row r="398" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="398" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A398" s="4" t="str">
         <f t="shared" si="6"/>
         <v>0041500404</v>
@@ -43719,7 +43728,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="399" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="399" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A399" s="4" t="str">
         <f t="shared" si="6"/>
         <v>0041500404</v>
@@ -43832,7 +43841,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="400" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="400" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A400" s="4" t="str">
         <f t="shared" si="6"/>
         <v>0041500404</v>
@@ -43928,7 +43937,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="401" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="401" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A401" s="4" t="str">
         <f t="shared" si="6"/>
         <v>0041500404</v>
@@ -44028,7 +44037,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="402" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="402" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A402" s="4" t="str">
         <f t="shared" si="6"/>
         <v>0041500404</v>
@@ -44141,7 +44150,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="403" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="403" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A403" s="4" t="str">
         <f t="shared" si="6"/>
         <v>0041500404</v>
@@ -44237,7 +44246,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="404" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="404" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A404" s="4" t="str">
         <f t="shared" si="6"/>
         <v>0041500404</v>
@@ -44348,7 +44357,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="405" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="405" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A405" s="4" t="str">
         <f t="shared" si="6"/>
         <v>0041500404</v>
@@ -44444,7 +44453,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="406" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="406" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A406" s="4" t="str">
         <f t="shared" si="6"/>
         <v>0041500404</v>
@@ -44555,7 +44564,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="407" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="407" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A407" s="4" t="str">
         <f t="shared" si="6"/>
         <v>0041500404</v>
@@ -44651,7 +44660,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="408" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="408" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A408" s="4" t="str">
         <f t="shared" si="6"/>
         <v>0041500404</v>
@@ -44762,7 +44771,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="409" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="409" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A409" s="4" t="str">
         <f t="shared" si="6"/>
         <v>0041500404</v>
@@ -44858,7 +44867,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="410" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="410" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A410" s="4" t="str">
         <f t="shared" si="6"/>
         <v>0041500404</v>
@@ -44950,7 +44959,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="411" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="411" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A411" s="4" t="str">
         <f t="shared" si="6"/>
         <v>0041500404</v>
@@ -45050,7 +45059,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="412" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="412" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A412" s="4" t="str">
         <f t="shared" si="6"/>
         <v>0041500404</v>
@@ -45161,7 +45170,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="413" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="413" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A413" s="4" t="str">
         <f t="shared" si="6"/>
         <v>0041500404</v>
@@ -45257,7 +45266,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="414" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="414" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A414" s="4" t="str">
         <f t="shared" si="6"/>
         <v>0041500404</v>
@@ -45357,7 +45366,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="415" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="415" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A415" s="4" t="str">
         <f t="shared" si="6"/>
         <v>0041500404</v>
@@ -45468,7 +45477,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="416" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="416" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A416" s="4" t="str">
         <f t="shared" si="6"/>
         <v>0041500404</v>
@@ -45581,7 +45590,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="417" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="417" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A417" s="4" t="str">
         <f t="shared" si="6"/>
         <v>0041500404</v>
@@ -45692,7 +45701,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="418" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="418" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A418" s="4" t="str">
         <f t="shared" si="6"/>
         <v>0041500404</v>
@@ -45788,7 +45797,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="419" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="419" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A419" s="4" t="str">
         <f t="shared" si="6"/>
         <v>0041500404</v>
@@ -45899,7 +45908,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="420" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="420" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A420" s="4" t="str">
         <f t="shared" si="6"/>
         <v>0041500404</v>
@@ -45991,7 +46000,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="421" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="421" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A421" s="4" t="str">
         <f t="shared" si="6"/>
         <v>0041500404</v>
@@ -46087,7 +46096,7 @@
       <c r="AQ421" s="4"/>
       <c r="AR421" s="4"/>
     </row>
-    <row r="422" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="422" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A422" s="4" t="str">
         <f t="shared" si="6"/>
         <v>0041500404</v>
@@ -46189,7 +46198,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="423" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="423" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A423" s="4" t="str">
         <f t="shared" si="6"/>
         <v>0041500404</v>
@@ -46300,7 +46309,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="424" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="424" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A424" s="4" t="str">
         <f t="shared" si="6"/>
         <v>0041500404</v>
@@ -46392,7 +46401,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="425" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="425" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A425" s="4" t="str">
         <f t="shared" si="6"/>
         <v>0041500404</v>
@@ -46494,7 +46503,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="426" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="426" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A426" s="4" t="str">
         <f t="shared" si="6"/>
         <v>0041500404</v>
@@ -46607,7 +46616,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="427" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="427" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A427" s="4" t="str">
         <f t="shared" si="6"/>
         <v>0041500404</v>
@@ -46720,7 +46729,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="428" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="428" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A428" s="4" t="str">
         <f t="shared" si="6"/>
         <v>0041500404</v>
@@ -46812,7 +46821,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="429" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="429" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A429" s="4" t="str">
         <f t="shared" si="6"/>
         <v>0041500404</v>
@@ -46904,7 +46913,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="430" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="430" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A430" s="4" t="str">
         <f t="shared" si="6"/>
         <v>0041500404</v>
@@ -47015,7 +47024,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="431" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="431" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A431" s="4" t="str">
         <f t="shared" si="6"/>
         <v>0041500404</v>
@@ -47111,7 +47120,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="432" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="432" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A432" s="4" t="str">
         <f t="shared" si="6"/>
         <v>0041500404</v>
@@ -47211,7 +47220,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="433" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="433" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A433" s="4" t="str">
         <f t="shared" si="6"/>
         <v>0041500404</v>
@@ -47322,7 +47331,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="434" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="434" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A434" s="4" t="str">
         <f t="shared" si="6"/>
         <v>0041500404</v>
@@ -47418,7 +47427,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="435" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="435" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A435" s="4" t="str">
         <f t="shared" si="6"/>
         <v>0041500404</v>
@@ -47518,7 +47527,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="436" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="436" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A436" s="4" t="str">
         <f t="shared" si="6"/>
         <v>0041500404</v>
@@ -47622,7 +47631,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="437" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="437" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A437" s="4" t="str">
         <f t="shared" si="6"/>
         <v>0041500404</v>
@@ -47726,7 +47735,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="438" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="438" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A438" s="4" t="str">
         <f t="shared" si="6"/>
         <v>0041500404</v>
@@ -47822,7 +47831,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="439" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="439" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A439" s="4" t="str">
         <f t="shared" si="6"/>
         <v>0041500404</v>
@@ -47935,7 +47944,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="440" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="440" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A440" s="4" t="str">
         <f t="shared" si="6"/>
         <v>0041500404</v>
@@ -48027,7 +48036,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="441" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="441" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A441" s="4" t="str">
         <f t="shared" si="6"/>
         <v>0041500404</v>
@@ -48127,7 +48136,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="442" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="442" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A442" s="4" t="str">
         <f t="shared" si="6"/>
         <v>0041500404</v>
@@ -48238,7 +48247,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="443" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="443" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A443" s="4" t="str">
         <f t="shared" si="6"/>
         <v>0041500404</v>
@@ -48330,7 +48339,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="444" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="444" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A444" s="4" t="str">
         <f t="shared" si="6"/>
         <v>0041500404</v>
@@ -48430,7 +48439,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="445" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="445" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A445" s="4" t="str">
         <f t="shared" si="6"/>
         <v>0041500404</v>
@@ -48530,7 +48539,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="446" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="446" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A446" s="4" t="str">
         <f t="shared" si="6"/>
         <v>0041500404</v>
@@ -48622,7 +48631,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="447" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="447" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A447" s="4" t="str">
         <f t="shared" si="6"/>
         <v>0041500404</v>
@@ -48722,7 +48731,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="448" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="448" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A448" s="4" t="str">
         <f t="shared" si="6"/>
         <v>0041500404</v>
@@ -48822,7 +48831,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="449" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="449" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A449" s="4" t="str">
         <f t="shared" si="6"/>
         <v>0041500404</v>
@@ -48926,7 +48935,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="450" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="450" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A450" s="4" t="str">
         <f t="shared" si="6"/>
         <v>0041500404</v>
@@ -49026,7 +49035,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="451" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="451" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A451" s="4" t="str">
         <f t="shared" ref="A451:A469" si="7">"0041500404"</f>
         <v>0041500404</v>
@@ -49130,7 +49139,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="452" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="452" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A452" s="4" t="str">
         <f t="shared" si="7"/>
         <v>0041500404</v>
@@ -49241,7 +49250,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="453" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="453" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A453" s="4" t="str">
         <f t="shared" si="7"/>
         <v>0041500404</v>
@@ -49341,7 +49350,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="454" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="454" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A454" s="4" t="str">
         <f t="shared" si="7"/>
         <v>0041500404</v>
@@ -49445,7 +49454,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="455" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="455" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A455" s="4" t="str">
         <f t="shared" si="7"/>
         <v>0041500404</v>
@@ -49549,7 +49558,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="456" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="456" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A456" s="4" t="str">
         <f t="shared" si="7"/>
         <v>0041500404</v>
@@ -49660,7 +49669,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="457" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="457" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A457" s="4" t="str">
         <f t="shared" si="7"/>
         <v>0041500404</v>
@@ -49760,7 +49769,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="458" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="458" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A458" s="4" t="str">
         <f t="shared" si="7"/>
         <v>0041500404</v>
@@ -49864,7 +49873,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="459" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="459" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A459" s="4" t="str">
         <f t="shared" si="7"/>
         <v>0041500404</v>
@@ -49968,7 +49977,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="460" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="460" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A460" s="4" t="str">
         <f t="shared" si="7"/>
         <v>0041500404</v>
@@ -50079,7 +50088,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="461" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="461" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A461" s="4" t="str">
         <f t="shared" si="7"/>
         <v>0041500404</v>
@@ -50179,7 +50188,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="462" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="462" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A462" s="4" t="str">
         <f t="shared" si="7"/>
         <v>0041500404</v>
@@ -50283,7 +50292,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="463" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="463" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A463" s="4" t="str">
         <f t="shared" si="7"/>
         <v>0041500404</v>
@@ -50387,7 +50396,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="464" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="464" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A464" s="4" t="str">
         <f t="shared" si="7"/>
         <v>0041500404</v>
@@ -50487,7 +50496,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="465" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="465" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A465" s="4" t="str">
         <f t="shared" si="7"/>
         <v>0041500404</v>
@@ -50587,7 +50596,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="466" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="466" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A466" s="4" t="str">
         <f t="shared" si="7"/>
         <v>0041500404</v>
@@ -50687,7 +50696,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="467" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="467" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A467" s="4" t="str">
         <f t="shared" si="7"/>
         <v>0041500404</v>
@@ -50791,7 +50800,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="468" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="468" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A468" s="4" t="str">
         <f t="shared" si="7"/>
         <v>0041500404</v>
@@ -50895,7 +50904,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="469" spans="1:44" x14ac:dyDescent="0.35">
+    <row r="469" spans="1:44" x14ac:dyDescent="0.15">
       <c r="A469" s="4" t="str">
         <f t="shared" si="7"/>
         <v>0041500404</v>
@@ -50986,36 +50995,35 @@
       <c r="AR469" s="4"/>
     </row>
   </sheetData>
-  <autoFilter ref="A2:AR469"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A2:A4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="129.59765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="129.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>562</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
         <v>564</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>563</v>
       </c>

</xml_diff>